<commit_message>
Updated R2 Pinout with control box code and descriptions.
</commit_message>
<xml_diff>
--- a/doc/Pinout-R2.xlsx
+++ b/doc/Pinout-R2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axl5646\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esn8034\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Frameside" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="69">
   <si>
     <t>Signal Name</t>
   </si>
@@ -118,6 +118,120 @@
   </si>
   <si>
     <t>Low Power Solenoid</t>
+  </si>
+  <si>
+    <t>Arming Chain</t>
+  </si>
+  <si>
+    <t>DrawInput</t>
+  </si>
+  <si>
+    <t>RetractInput</t>
+  </si>
+  <si>
+    <t>FireInput</t>
+  </si>
+  <si>
+    <t>LCDRegSelect</t>
+  </si>
+  <si>
+    <t>LCDEnable</t>
+  </si>
+  <si>
+    <t>41/43/45/47</t>
+  </si>
+  <si>
+    <t>RX0</t>
+  </si>
+  <si>
+    <t>TX0</t>
+  </si>
+  <si>
+    <t>LEDClock</t>
+  </si>
+  <si>
+    <t>LEDData</t>
+  </si>
+  <si>
+    <t>LCD Data, D4/D5/D6/D7</t>
+  </si>
+  <si>
+    <t>Emergency Stop button on frame</t>
+  </si>
+  <si>
+    <t>Emergency Stop button on control box</t>
+  </si>
+  <si>
+    <t>Front optical sensor (low: arrow present; high: arrow absent)</t>
+  </si>
+  <si>
+    <t>Rear optical sensor (low: arrow present; high: arrow absent)</t>
+  </si>
+  <si>
+    <t>SPI Analog to Digital Converter</t>
+  </si>
+  <si>
+    <t>Enable for the drawing linear actuator.</t>
+  </si>
+  <si>
+    <t>Direction for the drawing linear actuator.</t>
+  </si>
+  <si>
+    <t>Enable for the aiming linear actuator.</t>
+  </si>
+  <si>
+    <t>Direction for the aiming linear actuator.</t>
+  </si>
+  <si>
+    <t>Enable for the aiming gear motor.</t>
+  </si>
+  <si>
+    <t>Direction for the aiming gear motor.</t>
+  </si>
+  <si>
+    <t>High power fire solenoid used for firing.</t>
+  </si>
+  <si>
+    <t>Low power fire solenoid used to grab the string.</t>
+  </si>
+  <si>
+    <t>Receiving line for serial communications</t>
+  </si>
+  <si>
+    <t>Transmitting line for serial communications</t>
+  </si>
+  <si>
+    <t>Emergency stop button on the frame</t>
+  </si>
+  <si>
+    <t>Emergency stop button on the control box</t>
+  </si>
+  <si>
+    <t>Draw button on the control box</t>
+  </si>
+  <si>
+    <t>Retract button on the control box</t>
+  </si>
+  <si>
+    <t>Fire button on the control box</t>
+  </si>
+  <si>
+    <t>Combination of key, switch, and deadman button on the control box.</t>
+  </si>
+  <si>
+    <t>Enable for LCD display on control box</t>
+  </si>
+  <si>
+    <t>Register Select for LCD display on control box</t>
+  </si>
+  <si>
+    <t>Data pins for LCD display on control box.</t>
+  </si>
+  <si>
+    <t>Time until next fire information</t>
+  </si>
+  <si>
+    <t>Data output for LED shift registers.</t>
   </si>
 </sst>
 </file>
@@ -185,41 +299,80 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,370 +668,421 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="18">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>13</v>
       </c>
+      <c r="G2" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="8">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>11</v>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="8">
         <v>32</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="16">
         <v>51</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="16">
         <v>50</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="16">
         <v>52</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="16">
         <v>34</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="16">
         <v>36</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="16">
         <v>2</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="G11" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="16">
         <v>4</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="G12" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="16">
         <v>6</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="G13" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="7">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="16">
+        <v>8</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="G14" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="16">
         <v>10</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="G15" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="16">
         <v>12</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="G16" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="16">
         <v>38</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="G17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="B18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="16">
         <v>40</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>11</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -889,87 +1093,352 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D4" s="2">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="G4" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D5" s="2">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="G5" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5">
+        <v>37</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="A2:G1048576">
+    <sortCondition ref="D2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated pinout and sketch to free serial pin
The serial pins TX0 and RX0 are on Arduino pin 1 and 0 respectively, so
they can not be used by other components.
</commit_message>
<xml_diff>
--- a/doc/Pinout-R2.xlsx
+++ b/doc/Pinout-R2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="72">
   <si>
     <t>Signal Name</t>
   </si>
@@ -147,10 +147,16 @@
     <t>Low power fire solenoid used to grab the string.</t>
   </si>
   <si>
-    <t>ADC Reset</t>
-  </si>
-  <si>
-    <t>Reset for the analog to digital converter</t>
+    <t>Serial TX0</t>
+  </si>
+  <si>
+    <t>Serial transmission pin</t>
+  </si>
+  <si>
+    <t>Serial RX0</t>
+  </si>
+  <si>
+    <t>Serial receiving pin.</t>
   </si>
   <si>
     <t>RX0</t>
@@ -282,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -311,6 +317,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -337,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,6 +381,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -422,7 +443,7 @@
   <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
@@ -584,7 +605,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>25</v>
@@ -711,7 +732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -734,7 +755,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
@@ -781,28 +802,52 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -830,33 +875,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="10.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="6.85714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="15.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="6.00510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="15.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.85714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="15.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.00510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="15.7142857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="63.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -864,49 +909,49 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>46</v>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="12" t="n">
+      <c r="A3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>48</v>
+      <c r="E3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,8 +973,8 @@
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>49</v>
+      <c r="G4" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,128 +996,128 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>50</v>
+      <c r="G5" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="12" t="n">
+      <c r="A6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>52</v>
+      <c r="E6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="12" t="n">
+      <c r="A7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="n">
         <v>32</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>54</v>
+      <c r="E7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="12" t="n">
+      <c r="A8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="14" t="n">
         <v>37</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>56</v>
+      <c r="E8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="12" t="n">
+      <c r="A9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="14" t="n">
         <v>39</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>58</v>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="12" t="n">
+      <c r="D10" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>60</v>
+      <c r="E10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>61</v>
+      <c r="A11" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1080,7 +1125,7 @@
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12" t="n">
+      <c r="D11" s="14" t="n">
         <v>42</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1089,13 +1134,13 @@
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>62</v>
+      <c r="G11" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>63</v>
+      <c r="A12" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -1103,7 +1148,7 @@
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="12" t="n">
+      <c r="D12" s="14" t="n">
         <v>44</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1112,54 +1157,54 @@
       <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>64</v>
+      <c r="G12" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="A13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="12" t="n">
+      <c r="D13" s="14" t="n">
         <v>46</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>66</v>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="A14" s="14" t="s">
         <v>69</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added rotary encoder pins to pinout and sketch.
The R2 Pinout diagram and frameside sketch did not include pins for the
rotary encoder, which gives horizontal position data. Both have been
updated.
</commit_message>
<xml_diff>
--- a/doc/Pinout-R2.xlsx
+++ b/doc/Pinout-R2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="78">
   <si>
     <t>Signal Name</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Direction for the aiming gear motor.</t>
+  </si>
+  <si>
+    <t>Rotary Encoder PinA</t>
+  </si>
+  <si>
+    <t>Yes(3)</t>
+  </si>
+  <si>
+    <t>Interrupt Pin A on the rotary encoder.</t>
+  </si>
+  <si>
+    <t>Rotary Encoder PinB</t>
+  </si>
+  <si>
+    <t>Yes(2)</t>
+  </si>
+  <si>
+    <t>Interrupt Pin B on the rotary encoder.</t>
   </si>
   <si>
     <t>High Power Solenoid</t>
@@ -443,12 +461,12 @@
   <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9948979591837"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7142857142857"/>
@@ -755,7 +773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
@@ -763,93 +781,137 @@
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D14" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7" t="n">
         <v>38</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="7" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="9" t="n">
+      <c r="E17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="9" t="n">
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -910,7 +972,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>8</v>
@@ -928,12 +990,12 @@
         <v>10</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>8</v>
@@ -951,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +1036,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,12 +1059,12 @@
         <v>14</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>8</v>
@@ -1020,12 +1082,12 @@
         <v>10</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>8</v>
@@ -1043,12 +1105,12 @@
         <v>10</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>8</v>
@@ -1066,12 +1128,12 @@
         <v>10</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>8</v>
@@ -1089,12 +1151,12 @@
         <v>10</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>8</v>
@@ -1112,12 +1174,12 @@
         <v>10</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1135,12 +1197,12 @@
         <v>10</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -1158,12 +1220,12 @@
         <v>10</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>8</v>
@@ -1181,12 +1243,12 @@
         <v>10</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>8</v>
@@ -1195,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>10</v>
@@ -1204,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added initial ethernet communication to frameside arduino.
</commit_message>
<xml_diff>
--- a/doc/Pinout-R2.xlsx
+++ b/doc/Pinout-R2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="80">
   <si>
     <t>Signal Name</t>
   </si>
@@ -165,16 +165,22 @@
     <t>Low power fire solenoid used to grab the string.</t>
   </si>
   <si>
-    <t>Serial TX0</t>
-  </si>
-  <si>
-    <t>Serial transmission pin</t>
-  </si>
-  <si>
-    <t>Serial RX0</t>
-  </si>
-  <si>
-    <t>Serial receiving pin.</t>
+    <t>Ethernet Shield SD Select</t>
+  </si>
+  <si>
+    <t>SD Card Select on the Ethernet shield; this must be disabled.</t>
+  </si>
+  <si>
+    <t>Ethernet Shield W5100 Select</t>
+  </si>
+  <si>
+    <t>Wired Ethernet select on the Ethernet shield.</t>
+  </si>
+  <si>
+    <t>Ethernet Shield SPI Output</t>
+  </si>
+  <si>
+    <t>Required output for the Ethernet shield, per Arduino Ethernet Shield main page.</t>
   </si>
   <si>
     <t>RX0</t>
@@ -368,7 +374,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,11 +407,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,8 +462,8 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,7 +637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
@@ -646,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
@@ -727,7 +729,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -738,7 +740,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>25</v>
@@ -842,7 +844,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -869,22 +871,22 @@
       <c r="A18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="B18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -892,26 +894,50 @@
       <c r="A19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>53</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -937,33 +963,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.85714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="15.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.00510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="15.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="10.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="6.85714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="15.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="6.00510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="15.7142857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="63.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -971,49 +997,49 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="12" t="n">
+      <c r="A2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>54</v>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="14" t="n">
+      <c r="A3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>56</v>
+      <c r="E3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,8 +1061,8 @@
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>57</v>
+      <c r="G4" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,128 +1084,128 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>58</v>
+      <c r="G5" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="14" t="n">
+      <c r="A6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>60</v>
+      <c r="E6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="14" t="n">
+      <c r="A7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="13" t="n">
         <v>32</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>62</v>
+      <c r="E7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="14" t="n">
+      <c r="A8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="13" t="n">
         <v>37</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>64</v>
+      <c r="E8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14" t="n">
+      <c r="A9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="13" t="n">
         <v>39</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>66</v>
+      <c r="E9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="14" t="n">
+      <c r="A10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="13" t="n">
         <v>40</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>68</v>
+      <c r="E10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>69</v>
+      <c r="A11" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1187,7 +1213,7 @@
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="13" t="n">
         <v>42</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1196,13 +1222,13 @@
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>70</v>
+      <c r="G11" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>71</v>
+      <c r="A12" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -1210,7 +1236,7 @@
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="14" t="n">
+      <c r="D12" s="13" t="n">
         <v>44</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1219,54 +1245,54 @@
       <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>72</v>
+      <c r="G12" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="14" t="n">
+      <c r="A13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="13" t="n">
         <v>46</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>74</v>
+      <c r="E13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>77</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediate changes to frameside, C#, and tester classes
May need further editing; pushed now for battery issues.
</commit_message>
<xml_diff>
--- a/doc/Pinout-R2.xlsx
+++ b/doc/Pinout-R2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
   <si>
     <t>Signal Name</t>
   </si>
@@ -84,6 +84,9 @@
     <t>Analog</t>
   </si>
   <si>
+    <t>A2</t>
+  </si>
+  <si>
     <t>Feedback pin for the drawing linear actuator.</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
   </si>
   <si>
     <t>Aiming Linac Feedback Pin</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
   <si>
     <t>Feedback pin for the aiming linear actuator.</t>
@@ -462,8 +468,8 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,8 +607,8 @@
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="n">
-        <v>2</v>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
@@ -611,44 +617,44 @@
         <v>10</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
@@ -657,12 +663,12 @@
         <v>10</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>21</v>
@@ -670,8 +676,8 @@
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <v>5</v>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
@@ -680,41 +686,41 @@
         <v>10</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>8</v>
@@ -726,41 +732,41 @@
         <v>10</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="7" t="n">
         <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="7" t="n">
         <v>12</v>
@@ -772,12 +778,12 @@
         <v>10</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
@@ -786,21 +792,21 @@
         <v>9</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
@@ -809,27 +815,27 @@
         <v>9</v>
       </c>
       <c r="D15" s="7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7" t="n">
         <v>38</v>
@@ -841,18 +847,18 @@
         <v>10</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="7" t="n">
         <v>40</v>
@@ -864,18 +870,18 @@
         <v>10</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="8" t="n">
         <v>4</v>
@@ -887,18 +893,18 @@
         <v>10</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" s="8" t="n">
         <v>10</v>
@@ -910,18 +916,18 @@
         <v>10</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="8" t="n">
         <v>53</v>
@@ -933,7 +939,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -998,7 +1004,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>8</v>
@@ -1016,18 +1022,18 @@
         <v>10</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="13" t="n">
         <v>1</v>
@@ -1039,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1068,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,18 +1091,18 @@
         <v>14</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="13" t="n">
         <v>30</v>
@@ -1108,18 +1114,18 @@
         <v>10</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="13" t="n">
         <v>32</v>
@@ -1131,18 +1137,18 @@
         <v>10</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="13" t="n">
         <v>37</v>
@@ -1154,18 +1160,18 @@
         <v>10</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="13" t="n">
         <v>39</v>
@@ -1177,12 +1183,12 @@
         <v>10</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
@@ -1200,12 +1206,12 @@
         <v>10</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1223,12 +1229,12 @@
         <v>10</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -1246,12 +1252,12 @@
         <v>10</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>8</v>
@@ -1269,21 +1275,21 @@
         <v>10</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>10</v>
@@ -1292,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>